<commit_message>
Removed Requests for long press
</commit_message>
<xml_diff>
--- a/docs/SD Card Data Structure.xlsx
+++ b/docs/SD Card Data Structure.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily\Documents\GitHub\CAN-Logger-2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D0D30FE-D1B8-49CD-A25F-CCA319CA9DD7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CF7662-133E-42C2-A2EF-57353DC6EE09}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13965" xr2:uid="{EDF447FC-8B3D-46DE-9F1A-398DE83A960F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13965" activeTab="2" xr2:uid="{EDF447FC-8B3D-46DE-9F1A-398DE83A960F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SD Card Data Structure" sheetId="1" r:id="rId1"/>
+    <sheet name="CAN Frame Data Structure" sheetId="2" r:id="rId2"/>
+    <sheet name="EEPROM Map" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="79">
   <si>
     <t>Bytes</t>
   </si>
@@ -151,6 +153,123 @@
   </si>
   <si>
     <t>Can2 TEC</t>
+  </si>
+  <si>
+    <t>Current Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 | 1 | 2 </t>
+  </si>
+  <si>
+    <t>Corresponds to Can0, Can1, or Can2</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Number of seconds from the epoch (1970)</t>
+  </si>
+  <si>
+    <t>System Microseconds</t>
+  </si>
+  <si>
+    <t>The system microsecond counter when the CAN registers were read.</t>
+  </si>
+  <si>
+    <t>CAN Identifier</t>
+  </si>
+  <si>
+    <t>CAN ID with the Error Flags and Extended Flag, like Socket CAN</t>
+  </si>
+  <si>
+    <t>DLC</t>
+  </si>
+  <si>
+    <t>Data Length Code</t>
+  </si>
+  <si>
+    <t>Microseconds per second</t>
+  </si>
+  <si>
+    <t>Fractional seconds per tick of the Timestamp</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>Message Data Bytes padded with x0FF if not used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 </t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Can0 Bitrate Index</t>
+  </si>
+  <si>
+    <t>Bitrate Index</t>
+  </si>
+  <si>
+    <t>Can1 Bitrate Index</t>
+  </si>
+  <si>
+    <t>Can2 Bitrate Index</t>
+  </si>
+  <si>
+    <t>File ID. Each digit can be 0-9 or A-Z for a total of 36*3 = 46,656 files.</t>
+  </si>
+  <si>
+    <t>Logger Identifier of 2 uppercase letters</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>RES</t>
   </si>
 </sst>
 </file>
@@ -403,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,9 +558,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,16 +567,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -490,6 +602,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950AB3D3-75D5-4612-8050-A94890085CEE}">
   <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,126 +1006,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <v>0</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <v>1</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <v>2</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="13">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="13">
         <v>479</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H1" s="13">
         <v>480</v>
       </c>
-      <c r="I1" s="14">
+      <c r="I1" s="13">
         <v>481</v>
       </c>
-      <c r="J1" s="14">
+      <c r="J1" s="13">
         <v>482</v>
       </c>
-      <c r="K1" s="14">
+      <c r="K1" s="13">
         <v>483</v>
       </c>
-      <c r="L1" s="14">
+      <c r="L1" s="13">
         <v>484</v>
       </c>
-      <c r="M1" s="14">
+      <c r="M1" s="13">
         <v>485</v>
       </c>
-      <c r="N1" s="14">
+      <c r="N1" s="13">
         <v>486</v>
       </c>
-      <c r="O1" s="14">
+      <c r="O1" s="13">
         <v>487</v>
       </c>
-      <c r="P1" s="14">
+      <c r="P1" s="13">
         <v>488</v>
       </c>
-      <c r="Q1" s="14">
+      <c r="Q1" s="13">
         <v>489</v>
       </c>
-      <c r="R1" s="14">
+      <c r="R1" s="13">
         <v>490</v>
       </c>
-      <c r="S1" s="14">
+      <c r="S1" s="13">
         <v>491</v>
       </c>
-      <c r="T1" s="14">
+      <c r="T1" s="13">
         <v>492</v>
       </c>
-      <c r="U1" s="14">
+      <c r="U1" s="13">
         <v>493</v>
       </c>
-      <c r="V1" s="14">
+      <c r="V1" s="13">
         <v>494</v>
       </c>
-      <c r="W1" s="14">
+      <c r="W1" s="13">
         <v>495</v>
       </c>
-      <c r="X1" s="14">
+      <c r="X1" s="13">
         <v>496</v>
       </c>
-      <c r="Y1" s="14">
+      <c r="Y1" s="13">
         <v>497</v>
       </c>
-      <c r="Z1" s="14">
+      <c r="Z1" s="13">
         <v>498</v>
       </c>
-      <c r="AA1" s="14">
+      <c r="AA1" s="13">
         <v>499</v>
       </c>
-      <c r="AB1" s="14">
+      <c r="AB1" s="13">
         <v>500</v>
       </c>
-      <c r="AC1" s="14">
+      <c r="AC1" s="13">
         <v>501</v>
       </c>
-      <c r="AD1" s="14">
+      <c r="AD1" s="13">
         <v>502</v>
       </c>
-      <c r="AE1" s="14">
+      <c r="AE1" s="13">
         <v>503</v>
       </c>
-      <c r="AF1" s="14">
+      <c r="AF1" s="13">
         <v>504</v>
       </c>
-      <c r="AG1" s="14">
+      <c r="AG1" s="13">
         <v>505</v>
       </c>
-      <c r="AH1" s="14">
+      <c r="AH1" s="13">
         <v>506</v>
       </c>
-      <c r="AI1" s="14">
+      <c r="AI1" s="13">
         <v>507</v>
       </c>
-      <c r="AJ1" s="14">
+      <c r="AJ1" s="13">
         <v>508</v>
       </c>
-      <c r="AK1" s="14">
+      <c r="AK1" s="13">
         <v>509</v>
       </c>
-      <c r="AL1" s="14">
+      <c r="AL1" s="13">
         <v>510</v>
       </c>
-      <c r="AM1" s="16">
+      <c r="AM1" s="15">
         <v>511</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1032,10 +1213,10 @@
       </c>
       <c r="AK2" s="6"/>
       <c r="AL2" s="6"/>
-      <c r="AM2" s="18"/>
+      <c r="AM2" s="16"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="4" t="str">
@@ -1130,74 +1311,74 @@
       </c>
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
-      <c r="AM3" s="19" t="s">
+      <c r="AM3" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:39" s="2" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="21" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="23" t="s">
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24" t="s">
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="25"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="27" t="s">
+      <c r="W4" s="22"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="24" t="s">
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="27" t="s">
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="29"/>
-      <c r="AG4" s="24" t="s">
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="26"/>
-      <c r="AJ4" s="23" t="s">
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="AK4" s="23"/>
-      <c r="AL4" s="23"/>
-      <c r="AM4" s="30"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -1222,4 +1403,446 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68D2770-A69D-4575-8E49-25412A53F53A}">
+  <dimension ref="A1:Z4"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="31"/>
+    <col min="2" max="2" width="20.140625" style="31" customWidth="1"/>
+    <col min="3" max="6" width="5.7109375" style="31" customWidth="1"/>
+    <col min="7" max="10" width="7" style="31" customWidth="1"/>
+    <col min="11" max="14" width="7.42578125" style="31" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" style="31" customWidth="1"/>
+    <col min="16" max="18" width="7.85546875" style="31" customWidth="1"/>
+    <col min="19" max="27" width="4.28515625" style="31" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45">
+        <v>1</v>
+      </c>
+      <c r="D1" s="45">
+        <v>2</v>
+      </c>
+      <c r="E1" s="45">
+        <v>3</v>
+      </c>
+      <c r="F1" s="45">
+        <v>4</v>
+      </c>
+      <c r="G1" s="45">
+        <v>5</v>
+      </c>
+      <c r="H1" s="45">
+        <v>6</v>
+      </c>
+      <c r="I1" s="45">
+        <v>7</v>
+      </c>
+      <c r="J1" s="45">
+        <v>8</v>
+      </c>
+      <c r="K1" s="45">
+        <v>9</v>
+      </c>
+      <c r="L1" s="45">
+        <v>10</v>
+      </c>
+      <c r="M1" s="45">
+        <v>11</v>
+      </c>
+      <c r="N1" s="45">
+        <v>12</v>
+      </c>
+      <c r="O1" s="45">
+        <v>13</v>
+      </c>
+      <c r="P1" s="45">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="45">
+        <v>15</v>
+      </c>
+      <c r="R1" s="45">
+        <v>16</v>
+      </c>
+      <c r="S1" s="45">
+        <v>17</v>
+      </c>
+      <c r="T1" s="45">
+        <v>18</v>
+      </c>
+      <c r="U1" s="45">
+        <v>19</v>
+      </c>
+      <c r="V1" s="45">
+        <v>20</v>
+      </c>
+      <c r="W1" s="45">
+        <v>21</v>
+      </c>
+      <c r="X1" s="45">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="45">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="46">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y2" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z2" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="32">
+        <v>8</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="U3" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="V3" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="W3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z3" s="37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:Z4"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D47BF9-5D8C-4287-BE73-36659F6A543B}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="45">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45">
+        <v>1</v>
+      </c>
+      <c r="D1" s="45">
+        <v>2</v>
+      </c>
+      <c r="E1" s="45">
+        <v>3</v>
+      </c>
+      <c r="F1" s="45">
+        <v>4</v>
+      </c>
+      <c r="G1" s="45">
+        <v>5</v>
+      </c>
+      <c r="H1" s="45">
+        <v>6</v>
+      </c>
+      <c r="I1" s="45">
+        <v>7</v>
+      </c>
+      <c r="J1" s="45">
+        <v>8</v>
+      </c>
+      <c r="K1" s="45">
+        <v>9</v>
+      </c>
+      <c r="L1" s="45">
+        <v>10</v>
+      </c>
+      <c r="M1" s="48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="str">
+        <f>DEC2HEX(CODE(F2))</f>
+        <v>32</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="J3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>